<commit_message>
added header text for 17 species
</commit_message>
<xml_diff>
--- a/resources/Master_checklist.xlsx
+++ b/resources/Master_checklist.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4116" uniqueCount="1800">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4119" uniqueCount="1802">
   <si>
     <t>Total</t>
   </si>
@@ -5440,6 +5440,12 @@
   </si>
   <si>
     <t>Year-round</t>
+  </si>
+  <si>
+    <t>Locally common breeding resident</t>
+  </si>
+  <si>
+    <t>Very localised breeding resident and wanderer</t>
   </si>
 </sst>
 </file>
@@ -5791,8 +5797,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q453"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A373" workbookViewId="0">
-      <selection activeCell="A381" sqref="A381"/>
+    <sheetView tabSelected="1" topLeftCell="C363" workbookViewId="0">
+      <selection activeCell="G374" sqref="G374"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5833,11 +5839,11 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1">
         <f>(COUNTIF(G4:G376,"A"))</f>
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="H2" s="1">
         <f>(COUNTIF(G4:G376,"D"))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I2" s="1">
         <f>(COUNTIF(G4:G376,"E"))</f>
@@ -5932,6 +5938,9 @@
       <c r="J4" t="s">
         <v>1799</v>
       </c>
+      <c r="K4" t="s">
+        <v>1800</v>
+      </c>
       <c r="L4" t="s">
         <v>27</v>
       </c>
@@ -5973,6 +5982,9 @@
       <c r="G5" t="s">
         <v>1</v>
       </c>
+      <c r="K5" t="s">
+        <v>1801</v>
+      </c>
       <c r="L5" t="s">
         <v>27</v>
       </c>
@@ -6014,6 +6026,9 @@
       <c r="G6" t="s">
         <v>1</v>
       </c>
+      <c r="K6" t="s">
+        <v>1801</v>
+      </c>
       <c r="L6" t="s">
         <v>27</v>
       </c>
@@ -20371,7 +20386,7 @@
         <v>24</v>
       </c>
       <c r="G374" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L374" t="s">
         <v>27</v>

</xml_diff>